<commit_message>
cpp: webhooks route get namespace; py: pwd path to data.xlxs
</commit_message>
<xml_diff>
--- a/Programming/Labs/02/Python/data.xlsx
+++ b/Programming/Labs/02/Python/data.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44179.69807816335</v>
+        <v>44180.38637571139</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -469,7 +469,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -482,141 +482,15 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44179.69807816335</v>
+        <v>44180.38637571139</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>кока</t>
+          <t>подстаканник</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>44179.69807816335</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>тяжести</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>44179.69807816335</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>травы</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>44179.69807816335</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>эклеры</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>44179.69963751542</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>хлопья</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>44179.69963751542</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>вода</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>087195869592F40B2D56A3BF6C1EE441143EE5B967F0C68DC101E91E35736286</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>44179.69963751542</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>слиток</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>1000000</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>